<commit_message>
Acutualizacion plan de desarrollo
</commit_message>
<xml_diff>
--- a/03-Desarrollo/Interface_grafica/Cronograma.xlsx
+++ b/03-Desarrollo/Interface_grafica/Cronograma.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\proyecto-sicloud\03-Desarrollo\Interface_grafica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1D0984-B261-4DD4-BD31-17B9F4C36DCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D49D191-0F3F-40D1-8C0F-98103A75618D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{7D05BC6D-79FF-400D-ABDD-53A8E7B89697}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan de desarrollo" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -233,6 +233,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -242,20 +256,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,7 +582,7 @@
   <dimension ref="B1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +592,7 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -600,41 +600,41 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="6" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G3">
@@ -667,14 +667,14 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
@@ -691,40 +691,40 @@
       </c>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="2" t="s">
         <v>2</v>
       </c>
@@ -741,40 +741,40 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="2" t="s">
         <v>3</v>
       </c>
@@ -803,17 +803,17 @@
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -826,14 +826,14 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="2" t="s">
         <v>3</v>
       </c>
@@ -861,27 +861,27 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Docs: actualizacion de caso de usu extendido segun
</commit_message>
<xml_diff>
--- a/03-Desarrollo/Interface_grafica/Cronograma.xlsx
+++ b/03-Desarrollo/Interface_grafica/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\proyecto-sicloud\03-Desarrollo\Interface_grafica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8241D65-FD6C-42B3-A494-CCCF84E234FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A613DA64-49DA-4322-9783-F8A3078D4D8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{7D05BC6D-79FF-400D-ABDD-53A8E7B89697}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="50">
   <si>
     <t>ya</t>
   </si>
@@ -112,9 +112,6 @@
     <t>CCU012-InformeBodega</t>
   </si>
   <si>
-    <t>portal.php</t>
-  </si>
-  <si>
     <t>CU007-GenerarInformes_enlaces a los demas_informes</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">SICLOUD </t>
+  </si>
+  <si>
+    <t>CU0019-ServiciosPortal.php</t>
   </si>
 </sst>
 </file>
@@ -358,9 +358,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -370,6 +367,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,8 +689,8 @@
   <dimension ref="A2:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,85 +702,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="A2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="12">
         <f>COUNTIF(D5:D39,"Javier")</f>
         <v>13</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="12">
         <f>COUNTIF(D5:D39,"Daniel")</f>
         <v>5</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <f>COUNTIF(D5:D39,"Alejandro")</f>
         <v>5</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <f>COUNTIF(D5:D39,"David")</f>
         <v>6</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <f>COUNTIF(D5:D39,"Fabian")</f>
         <v>6</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <f>COUNTIF(B5:B39,"ya")</f>
         <v>25</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="12">
         <f>COUNTIF(B5:B39,"")</f>
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>0</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>0</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>0</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>0</v>
@@ -865,11 +865,11 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="9" t="s">
@@ -890,7 +890,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>0</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>0</v>
@@ -918,13 +918,13 @@
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
@@ -932,7 +932,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="9" t="s">
@@ -944,7 +944,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="9" t="s">
@@ -956,7 +956,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>0</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>0</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>0</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>0</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>0</v>
@@ -1026,13 +1026,13 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>1</v>
@@ -1040,13 +1040,13 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>2</v>
@@ -1054,13 +1054,13 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>3</v>
@@ -1068,13 +1068,13 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>3</v>
@@ -1082,13 +1082,13 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>3</v>
@@ -1096,13 +1096,13 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>3</v>
@@ -1110,13 +1110,13 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>3</v>
@@ -1124,13 +1124,13 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>3</v>
@@ -1138,13 +1138,13 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>3</v>
@@ -1152,13 +1152,13 @@
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>3</v>
@@ -1166,13 +1166,13 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>3</v>
@@ -1180,11 +1180,11 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>3</v>
@@ -1192,11 +1192,11 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>1</v>
@@ -1204,11 +1204,11 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>5</v>
@@ -1216,11 +1216,11 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>4</v>
@@ -1228,11 +1228,11 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>2</v>
@@ -1240,11 +1240,11 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Chore: Se agrega validacion de session en CU
</commit_message>
<xml_diff>
--- a/03-Desarrollo/Interface_grafica/Cronograma.xlsx
+++ b/03-Desarrollo/Interface_grafica/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\proyecto-sicloud\03-Desarrollo\Interface_grafica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496108F3-9BA6-48EE-9C50-AFDF605F3663}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D942CA2-351D-4754-B15E-D34FA2B5C6F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{7D05BC6D-79FF-400D-ABDD-53A8E7B89697}"/>
   </bookViews>
@@ -154,9 +154,6 @@
     <t>home</t>
   </si>
   <si>
-    <t>CU011-tablaVentas</t>
-  </si>
-  <si>
     <t>Rol-bodega</t>
   </si>
   <si>
@@ -182,6 +179,9 @@
   </si>
   <si>
     <t>CU0010-recuperarContrasena</t>
+  </si>
+  <si>
+    <t>CU0011-tablaVentas</t>
   </si>
 </sst>
 </file>
@@ -370,9 +370,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,6 +380,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,11 +699,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133BEB89-8072-48D1-A379-DCF06ACF145A}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10:E11"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,17 +712,17 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
@@ -745,10 +746,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="10">
         <f>COUNTIF(D5:D40,"Javier")</f>
         <v>13</v>
@@ -788,11 +789,11 @@
       <c r="C4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
@@ -802,11 +803,11 @@
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -816,7 +817,7 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -830,11 +831,11 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
@@ -844,11 +845,11 @@
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
@@ -858,11 +859,11 @@
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
@@ -872,12 +873,12 @@
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -885,12 +886,12 @@
       <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
@@ -898,11 +899,11 @@
       <c r="C12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
@@ -912,7 +913,7 @@
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -924,13 +925,13 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>29</v>
       </c>
@@ -940,7 +941,7 @@
       <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>2</v>
       </c>
     </row>
@@ -952,13 +953,13 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>29</v>
       </c>
@@ -966,7 +967,7 @@
       <c r="C17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>2</v>
       </c>
     </row>
@@ -978,7 +979,7 @@
       <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -992,11 +993,11 @@
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>29</v>
       </c>
@@ -1006,11 +1007,11 @@
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -1020,11 +1021,11 @@
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
@@ -1034,11 +1035,11 @@
       <c r="C22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>29</v>
       </c>
@@ -1048,25 +1049,25 @@
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
@@ -1076,11 +1077,11 @@
       <c r="C25" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>30</v>
       </c>
@@ -1090,11 +1091,11 @@
       <c r="C26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>30</v>
       </c>
@@ -1104,11 +1105,11 @@
       <c r="C27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
@@ -1118,11 +1119,11 @@
       <c r="C28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>30</v>
       </c>
@@ -1132,11 +1133,11 @@
       <c r="C29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>30</v>
       </c>
@@ -1146,11 +1147,11 @@
       <c r="C30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>30</v>
       </c>
@@ -1160,11 +1161,11 @@
       <c r="C31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
@@ -1174,11 +1175,11 @@
       <c r="C32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>30</v>
       </c>
@@ -1188,11 +1189,11 @@
       <c r="C33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>30</v>
       </c>
@@ -1202,31 +1203,31 @@
       <c r="C34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1236,50 +1237,56 @@
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="16" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B4:D39" xr:uid="{A409E96F-C6CE-4F66-9CEC-4881C18137B2}"/>
+  <autoFilter ref="B4:D40" xr:uid="{A409E96F-C6CE-4F66-9CEC-4881C18137B2}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Alejandro"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A2:D3"/>
   </mergeCells>

</xml_diff>